<commit_message>
Changed to Email Handler
- Removed Support for Weekends (Caused Date Issues)
- Added Support for Weekly (On Date of Registration)
- Refind the Email Process to speed it up
- Added Extensive Logging System
- Added More Try Catch to reduce errors
</commit_message>
<xml_diff>
--- a/Project (UiPath)/ToborInc-Files/ReportLocal.xlsx
+++ b/Project (UiPath)/ToborInc-Files/ReportLocal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA Workspace\SFIA Project 2\Project (UiPath)\ToborInc-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFD80B9-906C-494B-A8DF-68E080A145B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5F17A3-DC43-4CDD-9C4B-C5D9E7F98BE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18705" yWindow="7815" windowWidth="17700" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preformance Report (Process 1)" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="257">
   <si>
     <t>Date/Time</t>
   </si>
@@ -791,6 +791,12 @@
   </si>
   <si>
     <t>Successfully</t>
+  </si>
+  <si>
+    <t>Checking Email</t>
+  </si>
+  <si>
+    <t>No Emails have been found</t>
   </si>
 </sst>
 </file>
@@ -1109,9 +1115,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -1135,6 +1141,34 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>44011.144201388888</v>
+      </c>
+      <c r="B2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>44011.144201388888</v>
+      </c>
+      <c r="B3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" t="s">
+        <v>256</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1144,7 +1178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0670FE8E-5E75-4B80-A23D-8A45B49A2263}">
   <dimension ref="A1:D292"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>